<commit_message>
add satuan in barang
</commit_message>
<xml_diff>
--- a/peminjaman_barang/Data Peminjaman Barang.xlsx
+++ b/peminjaman_barang/Data Peminjaman Barang.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>No</t>
   </si>
@@ -44,13 +44,16 @@
     <t>Penanggung Jawab</t>
   </si>
   <si>
-    <t>Biro</t>
+    <t>Satuan Kerja</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
     <t>Komputer</t>
+  </si>
+  <si>
+    <t>2 Pack</t>
   </si>
   <si>
     <t>Acara</t>
@@ -473,26 +476,26 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
-        <v>2</v>
+      <c r="E2" t="s">
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -508,26 +511,26 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>